<commit_message>
nice manhattan plots for top 10 microbe traits
</commit_message>
<xml_diff>
--- a/data/Microbe_Strains.xlsx
+++ b/data/Microbe_Strains.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mike/Desktop/Labwork/Havelock_2019/HAVELOCK_BG/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{688940CA-81A9-4048-98E1-9C808AC2F637}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF6C0A4-1319-B540-A2DF-173DDA324949}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5080" yWindow="2800" windowWidth="28040" windowHeight="17440" xr2:uid="{C2740B86-CA7E-BB4E-AB3C-C6ECFA8B80CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="63">
   <si>
     <t>Archangium gephyra</t>
   </si>
@@ -90,9 +90,6 @@
     <t>Stenotrophomonas maltophilia</t>
   </si>
   <si>
-    <t>German collection of microorganisms</t>
-  </si>
-  <si>
     <t>Vicinamibacter silvestris</t>
   </si>
   <si>
@@ -127,6 +124,102 @@
   </si>
   <si>
     <t>Sphingobium herbicidovorans</t>
+  </si>
+  <si>
+    <t>tax_group</t>
+  </si>
+  <si>
+    <t>German_collection_of_microorganisms</t>
+  </si>
+  <si>
+    <t>trait</t>
+  </si>
+  <si>
+    <t>N_treatment</t>
+  </si>
+  <si>
+    <t>T6</t>
+  </si>
+  <si>
+    <t>stdN</t>
+  </si>
+  <si>
+    <t>T37</t>
+  </si>
+  <si>
+    <t>T54</t>
+  </si>
+  <si>
+    <t>lowN</t>
+  </si>
+  <si>
+    <t>T57</t>
+  </si>
+  <si>
+    <t>T128</t>
+  </si>
+  <si>
+    <t>T145</t>
+  </si>
+  <si>
+    <t>T39</t>
+  </si>
+  <si>
+    <t>T75</t>
+  </si>
+  <si>
+    <t>T97</t>
+  </si>
+  <si>
+    <t>T100</t>
+  </si>
+  <si>
+    <t>T130</t>
+  </si>
+  <si>
+    <t>T129</t>
+  </si>
+  <si>
+    <t>T83</t>
+  </si>
+  <si>
+    <t>T110</t>
+  </si>
+  <si>
+    <t>T38</t>
+  </si>
+  <si>
+    <t>T121</t>
+  </si>
+  <si>
+    <t>stdN_lowN</t>
+  </si>
+  <si>
+    <t>T137</t>
+  </si>
+  <si>
+    <t>T34</t>
+  </si>
+  <si>
+    <t>T33</t>
+  </si>
+  <si>
+    <t>T7</t>
+  </si>
+  <si>
+    <t>T28</t>
+  </si>
+  <si>
+    <t>T16</t>
+  </si>
+  <si>
+    <t>GWAS_signal</t>
+  </si>
+  <si>
+    <t>strong</t>
+  </si>
+  <si>
+    <t>messy</t>
   </si>
 </sst>
 </file>
@@ -142,12 +235,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -162,8 +261,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -478,178 +579,358 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B64CD61-3547-7844-8CA5-7C6DC139248C}">
-  <dimension ref="A3:B25"/>
+  <dimension ref="A1:E23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="1"/>
-    <col min="2" max="2" width="34" customWidth="1"/>
+    <col min="1" max="4" width="32" customWidth="1"/>
+    <col min="5" max="5" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="9" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s">
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>11</v>
-      </c>
-      <c r="B16" t="s">
+    <row r="15" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="B16" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="B17" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="E17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B19" t="s">
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>16</v>
-      </c>
-      <c r="B23" t="s">
+    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+    <row r="23" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E23" s="2" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>